<commit_message>
update site to 0.6.7
</commit_message>
<xml_diff>
--- a/vignettes/standardisation_outputs/exp1.xlsx
+++ b/vignettes/standardisation_outputs/exp1.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -383,6 +383,16 @@
           <t>p.value</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>conf.low</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>conf.high</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -402,6 +412,12 @@
       <c r="E2">
         <v>2.019078760549726E-50</v>
       </c>
+      <c r="F2">
+        <v>0.5404943604321496</v>
+      </c>
+      <c r="G2">
+        <v>0.6930403085996321</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -421,6 +437,12 @@
       <c r="E3">
         <v>3.744355231283194E-10</v>
       </c>
+      <c r="F3">
+        <v>-0.1734842019197602</v>
+      </c>
+      <c r="G3">
+        <v>-0.09139143722564977</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -440,6 +462,12 @@
       <c r="E4">
         <v>3.240605993050028E-31</v>
       </c>
+      <c r="F4">
+        <v>-0.3096297438804556</v>
+      </c>
+      <c r="G4">
+        <v>-0.2229285242962351</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -459,6 +487,12 @@
       <c r="E5">
         <v>2.842853991601156E-08</v>
       </c>
+      <c r="F5">
+        <v>-0.1657064096745759</v>
+      </c>
+      <c r="G5">
+        <v>-0.07968324298859122</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -478,6 +512,12 @@
       <c r="E6">
         <v>2.909064931938101E-06</v>
       </c>
+      <c r="F6">
+        <v>0.05961719515769731</v>
+      </c>
+      <c r="G6">
+        <v>0.1449152733077592</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -497,6 +537,12 @@
       <c r="E7">
         <v>0.5904347189151085</v>
       </c>
+      <c r="F7">
+        <v>-0.05771013484998045</v>
+      </c>
+      <c r="G7">
+        <v>0.03286243204005899</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -516,6 +562,12 @@
       <c r="E8">
         <v>0.5838817041941612</v>
       </c>
+      <c r="F8">
+        <v>-0.00169392465957928</v>
+      </c>
+      <c r="G8">
+        <v>0.0009545036779651839</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -535,6 +587,12 @@
       <c r="E9">
         <v>0.7615778275485744</v>
       </c>
+      <c r="F9">
+        <v>-0.03018175431607399</v>
+      </c>
+      <c r="G9">
+        <v>0.04122469103777791</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -554,6 +612,12 @@
       <c r="E10">
         <v>0.5758117527120532</v>
       </c>
+      <c r="F10">
+        <v>-0.05047951731765825</v>
+      </c>
+      <c r="G10">
+        <v>0.0280754315198984</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -573,6 +637,12 @@
       <c r="E11">
         <v>0.4169073940310739</v>
       </c>
+      <c r="F11">
+        <v>-0.02303032095436251</v>
+      </c>
+      <c r="G11">
+        <v>0.0555499096555235</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -591,6 +661,12 @@
       </c>
       <c r="E12">
         <v>0.5457901921411806</v>
+      </c>
+      <c r="F12">
+        <v>-0.05814971966688868</v>
+      </c>
+      <c r="G12">
+        <v>0.03076935272063646</v>
       </c>
     </row>
   </sheetData>

</xml_diff>